<commit_message>
removed Shraddhas test data from excel
</commit_message>
<xml_diff>
--- a/com.ElfBatch14/src/test/resources/testData.xlsx
+++ b/com.ElfBatch14/src/test/resources/testData.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C91BFF-C310-4A27-BD46-31699501EA1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
   </bookViews>
   <sheets>
-    <sheet name="Leads" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,79 +18,12 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
-  <si>
-    <t>Mr.</t>
-  </si>
-  <si>
-    <t>vishwa</t>
-  </si>
-  <si>
-    <t>bagoji</t>
-  </si>
-  <si>
-    <t>idrive</t>
-  </si>
-  <si>
-    <t>dev</t>
-  </si>
-  <si>
-    <t>bnvfvxdfvc@gmail.com</t>
-  </si>
-  <si>
-    <t>nbbb@gmail.com</t>
-  </si>
-  <si>
-    <t>www.abc.com</t>
-  </si>
-  <si>
-    <t>aaa</t>
-  </si>
-  <si>
-    <t>abcdef</t>
-  </si>
-  <si>
-    <t>ghijka</t>
-  </si>
-  <si>
-    <t>jkhkjhjkh</t>
-  </si>
-  <si>
-    <t>iuhyugj</t>
-  </si>
-  <si>
-    <t>mnjbghcfgxdfzdszszsd</t>
-  </si>
-  <si>
-    <t>rakshit</t>
-  </si>
-  <si>
-    <t>rashid</t>
-  </si>
-  <si>
-    <t>google</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -114,25 +46,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -410,103 +330,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A6:T8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" activeCellId="1" sqref="A7 D21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="8" max="8" width="20.109375" customWidth="1"/>
-    <col min="20" max="20" width="18" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="1">
-        <v>9999</v>
-      </c>
-      <c r="G6" s="1">
-        <v>9</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I6" s="3">
-        <v>99999999</v>
-      </c>
-      <c r="J6" s="4">
-        <v>9090897897</v>
-      </c>
-      <c r="K6" s="3">
-        <v>8888</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N6" t="s">
-        <v>8</v>
-      </c>
-      <c r="O6">
-        <v>777</v>
-      </c>
-      <c r="P6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>10</v>
-      </c>
-      <c r="R6" t="s">
-        <v>11</v>
-      </c>
-      <c r="S6" t="s">
-        <v>12</v>
-      </c>
-      <c r="T6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1" xr:uid="{C1C0C850-6AEC-4B52-BA79-9BB387385666}"/>
-    <hyperlink ref="L6" r:id="rId2" xr:uid="{9717E56B-5910-4FD3-A714-AE984346B149}"/>
-    <hyperlink ref="M6" r:id="rId3" xr:uid="{6837F30B-AC68-4098-851F-B952538677C8}"/>
-  </hyperlinks>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>